<commit_message>
Changed literally everything around the excel activities
It made everything so much easier
I don't know why I didn't do this in the first place
</commit_message>
<xml_diff>
--- a/week2/UiPath_RegExActivity/ApplicantInfo.xlsx
+++ b/week2/UiPath_RegExActivity/ApplicantInfo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\Batches\230206-UiPath-BNYM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ashen\Desktop\Revature\gavin-gilbert-code\week2\UiPath_RegExActivity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4C1746E-BC3A-4E79-99AD-9995AD80193C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEB1DAC6-29D3-44AA-9012-14590CC66C7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31065" yWindow="2100" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -446,19 +446,19 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.08984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -478,7 +478,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -494,8 +494,11 @@
       <c r="E2" t="s">
         <v>10</v>
       </c>
+      <c r="F2" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -511,8 +514,11 @@
       <c r="E3" t="s">
         <v>15</v>
       </c>
+      <c r="F3" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -528,8 +534,11 @@
       <c r="E4" t="s">
         <v>20</v>
       </c>
+      <c r="F4" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -545,8 +554,11 @@
       <c r="E5" t="s">
         <v>24</v>
       </c>
+      <c r="F5" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -558,6 +570,9 @@
       </c>
       <c r="D6" t="s">
         <v>29</v>
+      </c>
+      <c r="F6" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -712,9 +727,27 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A399F8E-2F26-4A9B-ADFC-CDECAF81AB28}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A399F8E-2F26-4A9B-ADFC-CDECAF81AB28}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="8281136c-3236-4060-8248-b02a7f3e9f10"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{08881C51-C8EA-4232-90FB-18F2EB429C8D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{08881C51-C8EA-4232-90FB-18F2EB429C8D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>